<commit_message>
lifo allocator and assets
</commit_message>
<xml_diff>
--- a/doc/img/plan de cuadros.xlsx
+++ b/doc/img/plan de cuadros.xlsx
@@ -200,13 +200,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -230,6 +223,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -697,93 +696,93 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1121,7 +1120,7 @@
   <dimension ref="B1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1160,430 +1159,430 @@
       </c>
     </row>
     <row r="3" spans="2:8">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="30" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="21" t="s">
+      <c r="D3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="13"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="23" t="s">
+      <c r="D4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="13"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="23" t="s">
+      <c r="D5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="13"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="23" t="s">
+      <c r="D6" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="16" thickBot="1">
-      <c r="B7" s="14"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="29" t="s">
+      <c r="D7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="16" thickTop="1">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="33" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="32" t="s">
+      <c r="D8" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="26" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="13"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="23" t="s">
+      <c r="D9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="13"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="23" t="s">
+      <c r="D10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="13"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="23" t="s">
+      <c r="D11" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="16" thickBot="1">
-      <c r="B12" s="16"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="35" t="s">
+      <c r="D12" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="29" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="16" thickTop="1">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="30" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="23" t="s">
+      <c r="D13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="13"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="23" t="s">
+      <c r="D14" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="2:8">
-      <c r="B15" s="13"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="23" t="s">
+      <c r="D15" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="13"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="23" t="s">
+      <c r="D16" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="16" thickBot="1">
-      <c r="B17" s="14"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="29" t="s">
+      <c r="D17" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="16" thickTop="1">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="33" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="32" t="s">
+      <c r="D18" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="26" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="13"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="23" t="s">
+      <c r="D19" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="13"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="23" t="s">
+      <c r="D20" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="2:8">
-      <c r="B21" s="13"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="23" t="s">
+      <c r="D21" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="16" thickBot="1">
-      <c r="B22" s="17"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="26" t="s">
+      <c r="D22" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="20" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1594,8 +1593,9 @@
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="B18:B22"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>